<commit_message>
able to create appointment and write to excel
</commit_message>
<xml_diff>
--- a/data/Appointment_List.xlsx
+++ b/data/Appointment_List.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zent-zaxux/IdeaProjects/SC2002/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A830963E-C4B0-5F40-A2C5-9D09D0C70581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{A830963E-C4B0-5F40-A2C5-9D09D0C70581}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="20120" yWindow="2900" windowWidth="28040" windowHeight="17440" xr2:uid="{EAE68897-7552-7543-82C3-4606EC839D89}"/>
+    <workbookView windowHeight="17440" windowWidth="28040" xWindow="20120" xr2:uid="{EAE68897-7552-7543-82C3-4606EC839D89}" yWindow="2900"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Doctor ID</t>
   </si>
@@ -87,12 +87,22 @@
   </si>
   <si>
     <t>A003</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>9:00 am</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -143,19 +153,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="18" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -172,10 +182,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -210,7 +220,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin panose="02110004020202020204" typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -262,7 +272,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin panose="02110004020202020204" typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -373,21 +383,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -404,7 +414,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -476,15 +486,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" name="Office Theme" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39DE2FE9-6033-CA4A-8CD2-53C7B3EEC0EE}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39DE2FE9-6033-CA4A-8CD2-53C7B3EEC0EE}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
@@ -492,9 +502,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="5" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="26" customWidth="1"/>
+    <col min="4" max="5" customWidth="true" width="17.33203125" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="14.0" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="26.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -580,7 +590,30 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="n">
+        <v>45595.0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
able to generate unique appointment ID
</commit_message>
<xml_diff>
--- a/data/Appointment_List.xlsx
+++ b/data/Appointment_List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zent-zaxux/IdeaProjects/SC2002/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hx/Documents/SC2002/OOP_Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{A830963E-C4B0-5F40-A2C5-9D09D0C70581}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{3DBA0CE3-A150-7E41-A5F8-F217F1FDF995}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView windowHeight="17440" windowWidth="28040" xWindow="20120" xr2:uid="{EAE68897-7552-7543-82C3-4606EC839D89}" yWindow="2900"/>
+    <workbookView windowHeight="17120" windowWidth="30240" xWindow="0" xr2:uid="{EAE68897-7552-7543-82C3-4606EC839D89}" yWindow="760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
@@ -89,7 +89,7 @@
     <t>A003</t>
   </si>
   <si>
-    <t>test</t>
+    <t>A004</t>
   </si>
   <si>
     <t>9:00 am</t>
@@ -497,14 +497,14 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="5" customWidth="true" width="17.33203125" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="14.0" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="26.0" collapsed="false"/>
+    <col min="4" max="5" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
patient able to display past outcome records, availability loader able to load outcome record
</commit_message>
<xml_diff>
--- a/data/Appointment_List.xlsx
+++ b/data/Appointment_List.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hx/Documents/SC2002/OOP_Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{3DBA0CE3-A150-7E41-A5F8-F217F1FDF995}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09910B80-A741-9244-BE63-28B341865F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="17120" windowWidth="30240" xWindow="0" xr2:uid="{EAE68897-7552-7543-82C3-4606EC839D89}" yWindow="760"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17120" xr2:uid="{EAE68897-7552-7543-82C3-4606EC839D89}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Doctor ID</t>
   </si>
@@ -96,13 +96,21 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>A005</t>
+  </si>
+  <si>
+    <t>COMPLETED</t>
+  </si>
+  <si>
+    <t>Health check up, all normal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -153,19 +161,20 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="18" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -182,10 +191,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -220,7 +229,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="02110004020202020204" typeface="Aptos Display"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -272,7 +281,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="02110004020202020204" typeface="Aptos Narrow"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -383,21 +392,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -414,7 +423,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -486,25 +495,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" name="Office Theme" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39DE2FE9-6033-CA4A-8CD2-53C7B3EEC0EE}">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39DE2FE9-6033-CA4A-8CD2-53C7B3EEC0EE}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="5" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="4" max="5" width="17.33203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -590,7 +599,7 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -603,8 +612,8 @@
       <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="n">
-        <v>45595.0</v>
+      <c r="E5">
+        <v>45595</v>
       </c>
       <c r="F5" t="s">
         <v>18</v>
@@ -613,7 +622,30 @@
         <v>19</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1">
+        <v>45595</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added whatsapp alert to patient & update appoinemt ID usage
</commit_message>
<xml_diff>
--- a/data/Appointment_List.xlsx
+++ b/data/Appointment_List.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hx/Documents/SC2002/OOP_Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09910B80-A741-9244-BE63-28B341865F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{298BCB54-F924-A243-A9DC-DDB5890DD965}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17120" xr2:uid="{EAE68897-7552-7543-82C3-4606EC839D89}"/>
+    <workbookView windowHeight="17120" windowWidth="30240" xWindow="0" xr2:uid="{EAE68897-7552-7543-82C3-4606EC839D89}" yWindow="760"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
   <si>
     <t>Doctor ID</t>
   </si>
@@ -44,18 +44,12 @@
     <t>Patient ID</t>
   </si>
   <si>
-    <t>A001</t>
-  </si>
-  <si>
     <t>D001</t>
   </si>
   <si>
     <t>P1001</t>
   </si>
   <si>
-    <t>A002</t>
-  </si>
-  <si>
     <t>D002</t>
   </si>
   <si>
@@ -86,31 +80,47 @@
     <t>CONFIRMED</t>
   </si>
   <si>
-    <t>A003</t>
-  </si>
-  <si>
-    <t>A004</t>
-  </si>
-  <si>
-    <t>9:00 am</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>A005</t>
-  </si>
-  <si>
     <t>COMPLETED</t>
   </si>
   <si>
     <t>Health check up, all normal</t>
+  </si>
+  <si>
+    <t>2:00 pm</t>
+  </si>
+  <si>
+    <t>05:00 pm</t>
+  </si>
+  <si>
+    <t>AP01</t>
+  </si>
+  <si>
+    <t>AP02</t>
+  </si>
+  <si>
+    <t>AP03</t>
+  </si>
+  <si>
+    <t>AP05</t>
+  </si>
+  <si>
+    <t>AP04</t>
+  </si>
+  <si>
+    <t>AP06</t>
+  </si>
+  <si>
+    <t>06:00 pm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -161,20 +171,20 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="18" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="19" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -191,10 +201,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -229,7 +239,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin panose="02110004020202020204" typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -281,7 +291,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin panose="02110004020202020204" typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -392,21 +402,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -423,7 +433,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -495,30 +505,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" name="Office Theme" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39DE2FE9-6033-CA4A-8CD2-53C7B3EEC0EE}">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39DE2FE9-6033-CA4A-8CD2-53C7B3EEC0EE}">
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="5" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -527,30 +537,30 @@
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1">
         <v>45592</v>
@@ -561,16 +571,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1">
         <v>45596</v>
@@ -581,16 +591,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1">
         <v>45595</v>
@@ -601,51 +611,51 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
       <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1">
         <v>45595</v>
       </c>
-      <c r="F5" t="s">
-        <v>18</v>
+      <c r="F5" s="4">
+        <v>0.41666666666666669</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="1">
-        <v>45595</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.41666666666666669</v>
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>45596</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>